<commit_message>
Implementa relatório de execução
</commit_message>
<xml_diff>
--- a/patic/core/media/exec/Execução PA MODELO 2019.xlsx
+++ b/patic/core/media/exec/Execução PA MODELO 2019.xlsx
@@ -14,7 +14,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Execução!$B$8:$I$8</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="256">
   <si>
     <t>Execução Plano de Aquisição de TIC 2019</t>
   </si>
@@ -127,9 +126,6 @@
     <t>msgStatusInvalido</t>
   </si>
   <si>
-    <t>RENOVAÇÃO DA PLATAFORMA DA SOLUÇÃO ECM (Projeto ePA) COM SUPORTE E MANUTENÇÃO EM 24 MESES</t>
-  </si>
-  <si>
     <t>Software de Prateleira</t>
   </si>
   <si>
@@ -142,16 +138,10 @@
     <t>Contratada/Adquirida</t>
   </si>
   <si>
-    <t xml:space="preserve">RENOVAÇÃO DE SERVIÇOS DE MAPEAMENTO E AUTOMAÇÃO DA PLATAFORMA DA SOLUÇÃO ECM PARA AMPLIAÇÃO DO PROJETO DE AUTOMAÇÃO DA PROCURADORIA ADMINISTRATIVA(Projeto ePA) </t>
-  </si>
-  <si>
     <t>Consultoria técnica especializada</t>
   </si>
   <si>
     <t>Serviço Não Comum</t>
-  </si>
-  <si>
-    <t>SUSTENTAÇÃO (MANUTENÇÃO ADAPTATIVA, EVOLUTIVA E CORRETIVA) DO SISTEMA DE AUTOMAÇÃO JUDICIAL DA PGE</t>
   </si>
   <si>
     <t>Manutenção de sistemas</t>
@@ -160,25 +150,13 @@
     <t>RENOVAÇÃO CONTRATAÇÃO DE EMPRESA PARA SERVIÇOS DE DESENVOLVIMENTO E TESTES DE SISTEMAS</t>
   </si>
   <si>
-    <t>ADEQUAÇÃO DAS SOLUÇÕES DE TIC INTERNAS ATRAVÉS DE DESENVOLVIMENTO OU MANUTENÇÃO DE SISTEMAS, AUTOMAÇÃO DE PROCESSOS E WEBSERVICES DE INTEGRAÇÃO (PRIMEIRA RENOVAÇÃO CONTRATUAL)</t>
-  </si>
-  <si>
     <t>Desenvolvimento e Manutenção de Sistemas</t>
-  </si>
-  <si>
-    <t>RENOVAÇÃO SERVIÇOS OBRIGATÓRIO PRODEB CONTEMPLA RENOVAÇÃO DE TODOS SERVIÇOS CONTRATADOS NAS ORDENS DE SERVIÇOS NO PROCESSO ATUAL</t>
-  </si>
-  <si>
-    <t>Processamento e Armazenamento (Prodeb)</t>
   </si>
   <si>
     <t>Prodeb Obrigatório</t>
   </si>
   <si>
     <t>AQUISIÇÃO DE MICROCOMPUTADORES INTERMEDIÁRIO</t>
-  </si>
-  <si>
-    <t>RENOVAÇÃO DO PARQUE EM GARANTIA E ADEQUAÇÃO DE NOVOS PROJETOS</t>
   </si>
   <si>
     <t>Microcomputador intermediário</t>
@@ -191,9 +169,6 @@
   </si>
   <si>
     <t>AQUISIÇÃO DE MICROCOMPUTADORES AVANCADOS</t>
-  </si>
-  <si>
-    <t>RENOVAÇÃO DO PARQUE EM GARANTIA E ADEQUAÇÃO DO PARQUE TECNOLOGICO AOS NOVOS PROJETOS ESTRATÉGICOS DA PGE</t>
   </si>
   <si>
     <t>Microcomputador avançado</t>
@@ -214,16 +189,10 @@
     <t>AQUISIÇÃO DE SWITCHES 24 PORTAS - EQUIPAMENTO DE CONECTIVIDADE</t>
   </si>
   <si>
-    <t>RENOVAÇÃO DO PARQUE EM GARANTIA E ADEQUAÇÃO DO PARQUE TECNOLOGICO PARA ATENDER NOVOS PROJETOS</t>
-  </si>
-  <si>
     <t>Switch</t>
   </si>
   <si>
     <t>AQUISIÇÃO DE SCANNER DE ALTO DESEMPENHO</t>
-  </si>
-  <si>
-    <t>EQUIPAMENTO PARA DIGITALIZAÇÃO DE GRANDES VOLUMES VISANDO PROJETO DE ePA (ECM) COM RECURSOS AVANÇADOS COMO MESA DIGITALIZADORA, DUPLA FACE E OCR</t>
   </si>
   <si>
     <t>Equipamentos para entrada de dados, inclusive scanners, leitores biométricos, catracas, de radiofrequência, de código de barras</t>
@@ -238,22 +207,10 @@
     <t>Impressão corporativa</t>
   </si>
   <si>
-    <t>RENOVAÇÃO CONTRATAÇÃO DE IMPRESSÃO CORPORATIVA PARA ATENDER POTENCIALMENTE ATÉ 10 REPRESENTAÇÕES REGIONAIS ; 55.000 FOLHAS</t>
-  </si>
-  <si>
-    <t>RENOVAÇÃO CONTRATAÇÃO DE IMPRESSÃO CORPORATIVA em 18/12/2018 PARA REPRESENTAÇÃO REGIONAL EM BRASÍLIA COM 5000 FOLHAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RENOVAÇÃO CONTRATAÇÃO DE IMPRESSÃO CORPORATIVA em 27/09/2018 PARA SALVADOR SAC BELLA VISTA ATENDENDO  26.500 FOLHAS </t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
     <t>Em estudo</t>
-  </si>
-  <si>
-    <t>AQUISIÇÃO DE FERRAMENTA DE BUSINESS INTELIGENCE PARA CONSTRUÇÃO INTERNA DE PAINEIS GERENCIAIS PARA ALTA GESTÃO</t>
   </si>
   <si>
     <t>Prodeb Não Obrigatório</t>
@@ -925,6 +882,9 @@
   </si>
   <si>
     <t>AQUISIÇÃO DE FERRAMENTA</t>
+  </si>
+  <si>
+    <t>Motivo XYZ</t>
   </si>
 </sst>
 </file>
@@ -2492,22 +2452,22 @@
     </row>
     <row r="9" spans="1:23" ht="60" customHeight="1">
       <c r="B9" s="33" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C9" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="E9" s="33" t="s">
         <v>33</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>34</v>
       </c>
       <c r="F9" s="34">
         <v>24</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="36">
         <v>1</v>
@@ -2516,7 +2476,7 @@
         <v>333000</v>
       </c>
       <c r="J9" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" s="52">
         <v>1</v>
@@ -2568,22 +2528,22 @@
     </row>
     <row r="10" spans="1:23" ht="60" customHeight="1">
       <c r="B10" s="33" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C10" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>37</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>39</v>
       </c>
       <c r="F10" s="34">
         <v>12</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="36">
         <v>1</v>
@@ -2592,7 +2552,7 @@
         <v>510000</v>
       </c>
       <c r="J10" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="52">
         <v>1</v>
@@ -2644,22 +2604,22 @@
     </row>
     <row r="11" spans="1:23" ht="60" customHeight="1">
       <c r="B11" s="33" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>40</v>
+        <v>255</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="34">
         <v>12</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="36">
         <v>1</v>
@@ -2668,7 +2628,7 @@
         <v>3400000</v>
       </c>
       <c r="J11" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K11" s="52">
         <v>1</v>
@@ -2720,22 +2680,22 @@
     </row>
     <row r="12" spans="1:23" ht="60" customHeight="1">
       <c r="B12" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="34">
         <v>12</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="38">
         <v>1</v>
@@ -2745,7 +2705,7 @@
         <v>1222000</v>
       </c>
       <c r="J12" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="52">
         <v>1</v>
@@ -2797,22 +2757,22 @@
     </row>
     <row r="13" spans="1:23" ht="60" customHeight="1">
       <c r="B13" s="35" t="s">
-        <v>266</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>45</v>
+        <v>252</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F13" s="34">
         <v>12</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="38">
         <v>1</v>
@@ -2822,7 +2782,7 @@
         <v>2160000</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K13" s="52">
         <v>1</v>
@@ -2874,22 +2834,22 @@
     </row>
     <row r="14" spans="1:23" ht="60" customHeight="1">
       <c r="B14" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F14" s="34">
         <v>36</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H14" s="38">
         <v>170</v>
@@ -2899,7 +2859,7 @@
         <v>629000</v>
       </c>
       <c r="J14" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K14" s="52">
         <v>150</v>
@@ -2952,22 +2912,22 @@
     </row>
     <row r="15" spans="1:23" ht="60" customHeight="1">
       <c r="B15" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F15" s="34">
         <v>36</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H15" s="38">
         <v>30</v>
@@ -2977,12 +2937,12 @@
         <v>141000</v>
       </c>
       <c r="J15" s="51" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K15" s="52"/>
       <c r="L15" s="53"/>
       <c r="M15" s="51" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="N15" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -3027,22 +2987,22 @@
     </row>
     <row r="16" spans="1:23" ht="60" customHeight="1">
       <c r="B16" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F16" s="34">
         <v>36</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H16" s="38">
         <v>30</v>
@@ -3052,12 +3012,12 @@
         <v>111000</v>
       </c>
       <c r="J16" s="51" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K16" s="52"/>
       <c r="L16" s="53"/>
       <c r="M16" s="51" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="N16" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -3102,22 +3062,22 @@
     </row>
     <row r="17" spans="2:23" ht="60" customHeight="1">
       <c r="B17" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F17" s="34">
         <v>36</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H17" s="38">
         <v>7</v>
@@ -3127,12 +3087,12 @@
         <v>42000</v>
       </c>
       <c r="J17" s="51" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K17" s="52"/>
       <c r="L17" s="53"/>
       <c r="M17" s="51" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="N17" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -3177,22 +3137,22 @@
     </row>
     <row r="18" spans="2:23" ht="60" customHeight="1">
       <c r="B18" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F18" s="34">
         <v>36</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H18" s="38">
         <v>5</v>
@@ -3202,12 +3162,12 @@
         <v>85000</v>
       </c>
       <c r="J18" s="51" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K18" s="52"/>
       <c r="L18" s="53"/>
       <c r="M18" s="51" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="N18" s="41" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -3252,22 +3212,22 @@
     </row>
     <row r="19" spans="2:23" ht="60" customHeight="1">
       <c r="B19" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>69</v>
+        <v>253</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F19" s="38">
         <v>12</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19" s="38">
         <v>12</v>
@@ -3276,7 +3236,7 @@
         <v>50000</v>
       </c>
       <c r="J19" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" s="52">
         <v>12</v>
@@ -3328,22 +3288,22 @@
     </row>
     <row r="20" spans="2:23" ht="60" customHeight="1">
       <c r="B20" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>70</v>
+        <v>253</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F20" s="38">
         <v>12</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" s="38">
         <v>12</v>
@@ -3352,7 +3312,7 @@
         <v>3800</v>
       </c>
       <c r="J20" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K20" s="52">
         <v>12</v>
@@ -3404,22 +3364,22 @@
     </row>
     <row r="21" spans="2:23" ht="60" customHeight="1">
       <c r="B21" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>71</v>
+        <v>253</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F21" s="38">
         <v>12</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" s="38">
         <v>12</v>
@@ -3428,7 +3388,7 @@
         <v>36225</v>
       </c>
       <c r="J21" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K21" s="52">
         <v>12</v>
@@ -3480,22 +3440,22 @@
     </row>
     <row r="22" spans="2:23" ht="60" customHeight="1">
       <c r="B22" s="45" t="s">
-        <v>268</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>74</v>
+        <v>254</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="D22" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="35" t="s">
         <v>33</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>34</v>
       </c>
       <c r="F22" s="38">
         <v>36</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H22" s="38">
         <v>1</v>
@@ -3504,7 +3464,7 @@
         <v>120000</v>
       </c>
       <c r="J22" s="51" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K22" s="52"/>
       <c r="L22" s="53"/>
@@ -56513,25 +56473,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.5">
       <c r="A1" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>22</v>
@@ -56549,195 +56509,195 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G3" s="26">
         <v>0</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G4" s="26">
         <v>0.05</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="18" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G5" s="26">
         <v>0.1</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="18" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="26">
         <v>0.15</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="18" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="G7" s="26">
         <v>0.2</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="E8" s="16" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G8" s="26">
         <v>0.25</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="16" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F9" s="55"/>
       <c r="G9" s="26">
         <v>0.3</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="19" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="26">
         <v>0.35</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="9" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="16" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F11" s="55"/>
       <c r="G11" s="26">
@@ -56747,13 +56707,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="10" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
       <c r="E12" s="16" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="F12" s="55"/>
       <c r="G12" s="26">
@@ -56763,13 +56723,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="19" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F13" s="55"/>
       <c r="G13" s="26">
@@ -56779,13 +56739,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="9" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="19" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F14" s="55"/>
       <c r="G14" s="26">
@@ -56795,13 +56755,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="10" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="16" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="F15" s="55"/>
       <c r="G15" s="26">
@@ -56811,13 +56771,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="8" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="19" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F16" s="55"/>
       <c r="G16" s="26">
@@ -56827,13 +56787,13 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="19" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F17" s="55"/>
       <c r="G17" s="26">
@@ -56842,13 +56802,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="F18" s="55"/>
       <c r="G18" s="26">
@@ -56857,13 +56817,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="19" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="F19" s="55"/>
       <c r="G19" s="26">
@@ -56872,13 +56832,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="11" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
       <c r="E20" s="19" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F20" s="55"/>
       <c r="G20" s="26">
@@ -56887,13 +56847,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="19" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F21" s="55"/>
       <c r="G21" s="26">
@@ -56902,13 +56862,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="10" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="19" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="26">
@@ -56917,13 +56877,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="19" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="F23" s="55"/>
       <c r="G23" s="26">
@@ -56932,111 +56892,111 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="19" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F24" s="55"/>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
       <c r="E25" s="19" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F25" s="55"/>
       <c r="G25" s="55"/>
     </row>
     <row r="26" spans="1:7" ht="25.5">
       <c r="A26" s="8" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
       <c r="E26" s="19" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F26" s="55"/>
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
       <c r="E27" s="19" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F27" s="55"/>
       <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="19" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="F28" s="55"/>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="19" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F29" s="55"/>
       <c r="G29" s="55"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="19" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F30" s="55"/>
       <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="19" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="F31" s="55"/>
       <c r="G31" s="55"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
@@ -57049,337 +57009,337 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="19" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
       <c r="E34" s="19" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="10" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
       <c r="E35" s="19" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="8" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="19" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="8" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="19" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="8" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="19" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="8" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="19" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="8" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
       <c r="E40" s="19" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
       <c r="E41" s="19" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
       <c r="D42" s="20"/>
       <c r="E42" s="19" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
       <c r="E43" s="19" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.5">
       <c r="A44" s="7" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="19" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="25.5">
       <c r="A45" s="12" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
       <c r="E45" s="19" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="10" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
       <c r="E46" s="19" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="19" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="25.5">
       <c r="A48" s="6" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
       <c r="E48" s="19" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="38.25">
       <c r="A49" s="6" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="19" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
       <c r="E50" s="19" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="20"/>
       <c r="E51" s="19" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
       <c r="E52" s="19" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="10" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
       <c r="E53" s="19" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
       <c r="E54" s="19" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="6" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
       <c r="D55" s="20"/>
       <c r="E55" s="19" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
       <c r="E56" s="19" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="9" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
       <c r="D57" s="20"/>
       <c r="E57" s="19" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="10" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
       <c r="E58" s="19" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="9" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
       <c r="D59" s="20"/>
       <c r="E59" s="19" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="10" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
       <c r="D60" s="20"/>
       <c r="E60" s="19" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="7" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
       <c r="D61" s="20"/>
       <c r="E61" s="19" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="8" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
       <c r="E62" s="19" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="7" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B63" s="20"/>
       <c r="C63" s="20"/>
@@ -57388,7 +57348,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B64" s="20"/>
       <c r="C64" s="20"/>
@@ -57397,287 +57357,287 @@
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="8" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="8" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="8" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="8" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="8" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="8" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="6" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="5" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="9" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="10" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="10" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="10" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="10" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="10" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="11" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="13" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="25.5">
       <c r="A83" s="11" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="8" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="8" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="8" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="14" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="9" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="10" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="14" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="14" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="12" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="14" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="5" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="8" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="8" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="5" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="5" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="5" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="8" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="7" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="8" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" s="5" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="6" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" s="9" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="10" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="5" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="8" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="14" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="8" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="6" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="9" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="10" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="8" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="9" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="10" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>